<commit_message>
Ajout documents présentation B&R et mise à jour du doc Nomenclature
</commit_message>
<xml_diff>
--- a/Documents/Nomenclature.xlsx
+++ b/Documents/Nomenclature.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://stfelixlasalle-my.sharepoint.com/personal/jean-remy_dion_stfelixlasalle_fr/Documents/Documents/GitHub/SN2_SFL4Manitou_23/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{34256D1A-387F-49E0-AA17-5F2A38CD2867}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="119" documentId="8_{34256D1A-387F-49E0-AA17-5F2A38CD2867}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A8BB7395-5795-404F-AEA4-DED525B075EE}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{A6D686BF-90D5-45E2-8742-EE7D7C910ECC}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
     <t>Nomenclature</t>
   </si>
@@ -78,7 +78,112 @@
     <t>Ecran tactile FT50</t>
   </si>
   <si>
-    <t>Processeur : ARM  Cortex-A9 4 cœurs | 800 MHz</t>
+    <t>Processeur : ARM  Cortex-A9 4 cœurs | 800 MHz
+DRAM : 2GB
+Flash : 512 MB
+Interfaces : 
+    - 1x Ethernet
+    - 1x USB 2.0
+Diagonale : 15,6 Pouces
+Résolution : 1366 x 768
+Couleurs : 16 millions
+Rétroéclairage : LED</t>
+  </si>
+  <si>
+    <t>4PP045.0571-062</t>
+  </si>
+  <si>
+    <t>Power Panel 45</t>
+  </si>
+  <si>
+    <t>Processeur : ELaN SC520 | 100 MHz
+DRAM : 64MB
+SRaM : 32 KB 
+Interfaces : 
+    - 1x Ethernet
+    - 2x USB 2.0
+    - 1x X2X Link Master
+Diagonale : 5,7 Pouces
+Résolution : 203 x 145 mm
+Couleurs : 256
+Rétroéclairage : LCD</t>
+  </si>
+  <si>
+    <t>X90CA100.02-00</t>
+  </si>
+  <si>
+    <t>X90 mobile wiring harness starter set for CMC header</t>
+  </si>
+  <si>
+    <t>3x cables : 
+    - 1x cable femelle X1.A
+    - 1x cable femelle X1.B
+    - 1x cable femelle X1.C</t>
+  </si>
+  <si>
+    <t>X67CAOE41.0020</t>
+  </si>
+  <si>
+    <t>Powerlink / Ethernet connection
+cable RJ45 vers M12</t>
+  </si>
+  <si>
+    <t>1x Powerlink / Ethernet connection
+cable RJ45 vers M12
+4 Pins
+Longueur : 2m</t>
+  </si>
+  <si>
+    <t>6ACCMA11.0300-000</t>
+  </si>
+  <si>
+    <t>FT50 pied d'écran</t>
+  </si>
+  <si>
+    <t>1x FT50 pied d'écran
+Dimensions : 
+    - Largeur : 168,2 mm
+    - Longueur : 158,1 mm
+    -  Hauteur : 282,1 mm</t>
+  </si>
+  <si>
+    <t>6COPOE.0000-00</t>
+  </si>
+  <si>
+    <t>Power Of Ethernet (POE)</t>
+  </si>
+  <si>
+    <t>LEDs : 
+    - Port d'entrée Ethernet 10/100
+    - Port de sortie Ethernet 10/100 PoE
+   - 3x LEDs pour les diagnostiques
+1x connexion réseau (RJ45)
+1x Sortie 24 VDC 
+1x PoE (RJ45)</t>
+  </si>
+  <si>
+    <t>6CAPFT.0030-02</t>
+  </si>
+  <si>
+    <t>FT50 cable de connexion Ethernet + écran</t>
+  </si>
+  <si>
+    <t>1x RJ45 (male)
+1x USB (femele)
+Longueurs : 
+    - PoE : 3m
+    - USB : 1m</t>
+  </si>
+  <si>
+    <t>0PS1100.1</t>
+  </si>
+  <si>
+    <t>Power Supply</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alimentation 24 VDC
+Entrée 100 à 240 VAC
+</t>
   </si>
 </sst>
 </file>
@@ -141,16 +246,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -175,6 +277,13 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -279,6 +388,348 @@
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1762125</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>1790700</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Image 1" descr="B&amp;R 4PP065.0571-X74 HMI at Rs 13000 in Bhavnagar | ID: 22096991333">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E3D05CB5-F012-7D28-7D31-BCAE56B83662}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="600075" y="6534150"/>
+          <a:ext cx="1619250" cy="1619250"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>752475</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1390739</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>2457792</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Image 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8D4468CC-621A-9AF0-64A7-527DC31FB39B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1209675" y="9906000"/>
+          <a:ext cx="638264" cy="2448267"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1828518</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>1447800</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="11" name="Image 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0B52D417-765D-4209-A1D0-72F013EDECFB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="514350" y="4657725"/>
+          <a:ext cx="1771368" cy="1362075"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>142876</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>2309892</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>1219200</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="12" name="Image 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E748CDC9-BF37-B43E-9414-EFECD83F8E7A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="600076" y="6343650"/>
+          <a:ext cx="2167016" cy="1028700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>85725</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>2111952</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>1495425</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="13" name="Image 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F4FCE688-E7E8-4B59-83DB-D14AFB45794F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="542925" y="12773025"/>
+          <a:ext cx="2026227" cy="1333500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>123826</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>295276</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>2105026</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>575304</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="14" name="Image 13">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DA74C1BA-86BE-4CA1-996E-32C54EB2933C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="581026" y="14563726"/>
+          <a:ext cx="1981200" cy="280028"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>302559</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>78441</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>2226609</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>2452407</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="15" name="Image 14" descr="B&amp;R: 0PS1100.1 – PTS – Technology">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E3E4BF10-D089-9CE4-8A36-DF2FD0525733}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="762000" y="15262412"/>
+          <a:ext cx="1924050" cy="2373966"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
       </xdr:spPr>
     </xdr:pic>
     <xdr:clientData/>
@@ -585,270 +1036,312 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0129D009-AB3C-49A2-9C0B-FD70C9CF620F}">
   <dimension ref="B1:I31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6.85546875" style="2" customWidth="1"/>
-    <col min="2" max="2" width="32" style="2" customWidth="1"/>
+    <col min="2" max="2" width="35.42578125" style="2" customWidth="1"/>
     <col min="3" max="3" width="18.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="28.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30.140625" style="2" customWidth="1"/>
     <col min="5" max="5" width="43.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.42578125" style="9"/>
+    <col min="6" max="6" width="11.42578125" style="8"/>
     <col min="7" max="16384" width="11.42578125" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
     </row>
     <row r="2" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B2" s="4"/>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
-      <c r="I2" s="4"/>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
     </row>
     <row r="3" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="G3" s="4"/>
-      <c r="H3" s="4"/>
-      <c r="I3" s="4"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="E4" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="10" t="s">
+      <c r="F4" s="9" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="5" spans="2:9" ht="135" x14ac:dyDescent="0.25">
       <c r="B5" s="1"/>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="8" t="s">
+      <c r="D5" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="7" t="s">
+      <c r="E5" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="F5" s="11">
+      <c r="F5" s="10">
         <v>702.9</v>
       </c>
     </row>
-    <row r="6" spans="2:9" ht="126" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:9" ht="165" x14ac:dyDescent="0.25">
       <c r="B6" s="1"/>
       <c r="C6" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="D6" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="E6" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="F6" s="11"/>
-    </row>
-    <row r="7" spans="2:9" ht="126" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="11"/>
+      <c r="F6" s="10"/>
+    </row>
+    <row r="7" spans="2:9" ht="124.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="12"/>
+      <c r="C7" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="F7" s="10"/>
     </row>
     <row r="8" spans="2:9" ht="126" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="11"/>
-    </row>
-    <row r="9" spans="2:9" ht="126" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C8" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="F8" s="10"/>
+    </row>
+    <row r="9" spans="2:9" ht="168.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="11"/>
-    </row>
-    <row r="10" spans="2:9" ht="126" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C9" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="F9" s="10"/>
+    </row>
+    <row r="10" spans="2:9" ht="213.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="11"/>
-    </row>
-    <row r="11" spans="2:9" ht="126" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C10" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="F10" s="10"/>
+    </row>
+    <row r="11" spans="2:9" ht="130.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="11"/>
-    </row>
-    <row r="12" spans="2:9" ht="126" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C11" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="F11" s="10"/>
+    </row>
+    <row r="12" spans="2:9" ht="72.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="11"/>
-    </row>
-    <row r="13" spans="2:9" ht="126" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="11"/>
+      <c r="C12" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F12" s="10"/>
+    </row>
+    <row r="13" spans="2:9" ht="202.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="12"/>
+      <c r="C13" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="F13" s="10"/>
     </row>
     <row r="14" spans="2:9" ht="126" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
-      <c r="F14" s="11"/>
+      <c r="F14" s="10"/>
     </row>
     <row r="15" spans="2:9" ht="126" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
-      <c r="F15" s="11"/>
+      <c r="F15" s="10"/>
     </row>
     <row r="16" spans="2:9" ht="126" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
-      <c r="F16" s="11"/>
+      <c r="F16" s="10"/>
     </row>
     <row r="17" spans="2:6" ht="126" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
-      <c r="F17" s="11"/>
+      <c r="F17" s="10"/>
     </row>
     <row r="18" spans="2:6" ht="126" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
-      <c r="F18" s="11"/>
+      <c r="F18" s="10"/>
     </row>
     <row r="19" spans="2:6" ht="126" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
-      <c r="F19" s="11"/>
+      <c r="F19" s="10"/>
     </row>
     <row r="20" spans="2:6" ht="126" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
-      <c r="F20" s="11"/>
+      <c r="F20" s="10"/>
     </row>
     <row r="21" spans="2:6" ht="126" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
-      <c r="F21" s="11"/>
+      <c r="F21" s="10"/>
     </row>
     <row r="22" spans="2:6" ht="126" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
-      <c r="F22" s="11"/>
+      <c r="F22" s="10"/>
     </row>
     <row r="23" spans="2:6" ht="126" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
-      <c r="F23" s="11"/>
+      <c r="F23" s="10"/>
     </row>
     <row r="24" spans="2:6" ht="126" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
       <c r="E24" s="1"/>
-      <c r="F24" s="11"/>
+      <c r="F24" s="10"/>
     </row>
     <row r="25" spans="2:6" ht="126" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
-      <c r="F25" s="11"/>
+      <c r="F25" s="10"/>
     </row>
     <row r="26" spans="2:6" ht="126" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
       <c r="E26" s="1"/>
-      <c r="F26" s="11"/>
+      <c r="F26" s="10"/>
     </row>
     <row r="27" spans="2:6" ht="126" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
       <c r="E27" s="1"/>
-      <c r="F27" s="11"/>
+      <c r="F27" s="10"/>
     </row>
     <row r="28" spans="2:6" ht="126" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
       <c r="E28" s="1"/>
-      <c r="F28" s="11"/>
+      <c r="F28" s="10"/>
     </row>
     <row r="29" spans="2:6" ht="126" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
       <c r="D29" s="1"/>
       <c r="E29" s="1"/>
-      <c r="F29" s="11"/>
+      <c r="F29" s="10"/>
     </row>
     <row r="30" spans="2:6" ht="126" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
       <c r="D30" s="1"/>
       <c r="E30" s="1"/>
-      <c r="F30" s="11"/>
+      <c r="F30" s="10"/>
     </row>
     <row r="31" spans="2:6" ht="126" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
       <c r="D31" s="1"/>
       <c r="E31" s="1"/>
-      <c r="F31" s="11"/>
+      <c r="F31" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>